<commit_message>
FIrst SetUP Project Commit
</commit_message>
<xml_diff>
--- a/src/test/java/com/TSBFramewor/swati/testData/TSBTradeTestdata.xlsx
+++ b/src/test/java/com/TSBFramewor/swati/testData/TSBTradeTestdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hphadas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hphadas\utitlity\partT\simple-selenium\TSBBankAutoFrameWork_swati\src\test\java\com\TSBFramewor\swati\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B649DFF3-3E58-4E03-8E84-534C4481F36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F0646-0AAD-4D2F-B21A-16466274EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1695" windowWidth="29040" windowHeight="15720" xr2:uid="{0A911388-B2D9-4E01-A36D-BE1341E2ABCA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +35,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Tom123</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>John123</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -46,15 +69,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +91,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +428,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37512547-F56D-473F-9540-CEE53D95D5A2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>